<commit_message>
Update Bank Deposit data - 2025-12-23T09:35:08.799Z
</commit_message>
<xml_diff>
--- a/Bank_Deposit.xlsx
+++ b/Bank_Deposit.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -540,9 +540,124 @@
         <v>2025-12-23</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>02-12-2025</v>
+      </c>
+      <c r="B7" t="str">
+        <v>010965012-Medha Sub Division Office Coll.</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D7" t="str">
+        <v>2025-12-03</v>
+      </c>
+      <c r="E7">
+        <v>8770</v>
+      </c>
+      <c r="F7" t="str">
+        <v>दिनांक __ रोजी रविवार असल्याने जमा झालेली रक्कम ही सोमवार दिनांक 03.12.2025 रोजी बँकेमध्ये भरणा करण्यात आली.</v>
+      </c>
+      <c r="G7" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>02-12-2025</v>
+      </c>
+      <c r="B8" t="str">
+        <v>010965012-Medha Sub Division Office Coll.</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="D8" t="str">
+        <v/>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="str">
+        <v>दिनांक __ रोजी रविवार असल्याने जमा झालेली रक्कम ही सोमवार दिनांक 03.12.2025 रोजी बँकेमध्ये भरणा करण्यात आली.</v>
+      </c>
+      <c r="G8" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>02-12-2025</v>
+      </c>
+      <c r="B9" t="str">
+        <v>010965012-Medha Sub Division Office Coll.</v>
+      </c>
+      <c r="C9" t="str">
+        <v>NEFT</v>
+      </c>
+      <c r="D9" t="str">
+        <v/>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="str">
+        <v>दिनांक __ रोजी रविवार असल्याने जमा झालेली रक्कम ही सोमवार दिनांक 03.12.2025 रोजी बँकेमध्ये भरणा करण्यात आली.</v>
+      </c>
+      <c r="G9" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>02-12-2025</v>
+      </c>
+      <c r="B10" t="str">
+        <v>010965012-Medha Sub Division Office Coll.</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Total</v>
+      </c>
+      <c r="D10" t="str">
+        <v/>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="str">
+        <v>दिनांक __ रोजी रविवार असल्याने जमा झालेली रक्कम ही सोमवार दिनांक 03.12.2025 रोजी बँकेमध्ये भरणा करण्यात आली.</v>
+      </c>
+      <c r="G10" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>02-12-2025</v>
+      </c>
+      <c r="B11" t="str">
+        <v>010965012-Medha Sub Division Office Coll.</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D11" t="str">
+        <v/>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="str">
+        <v>दिनांक 02.12.2025 रोजी रविवार असल्याने जमा झालेली रक्कम ही सोमवार दिनांक 03.12.2025 रोजी बँकेमध्ये भरणा करण्यात आली.</v>
+      </c>
+      <c r="G11" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Bank Deposit data - 2025-12-23T09:38:37.493Z
</commit_message>
<xml_diff>
--- a/Bank_Deposit.xlsx
+++ b/Bank_Deposit.xlsx
@@ -557,7 +557,7 @@
         <v>8770</v>
       </c>
       <c r="F7" t="str">
-        <v>दिनांक __ रोजी रविवार असल्याने जमा झालेली रक्कम ही सोमवार दिनांक 03.12.2025 रोजी बँकेमध्ये भरणा करण्यात आली.</v>
+        <v>दिनांक 02.12.2025 रोजी रविवार असल्याने जमा झालेली रक्कम ही सोमवार दिनांक 03.12.2025 रोजी बँकेमध्ये भरणा करण्यात आली.</v>
       </c>
       <c r="G7" t="str">
         <v>2025-12-23</v>
@@ -571,7 +571,7 @@
         <v>010965012-Medha Sub Division Office Coll.</v>
       </c>
       <c r="C8" t="str">
-        <v>Cheque</v>
+        <v>Cash</v>
       </c>
       <c r="D8" t="str">
         <v/>
@@ -580,7 +580,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="str">
-        <v>दिनांक __ रोजी रविवार असल्याने जमा झालेली रक्कम ही सोमवार दिनांक 03.12.2025 रोजी बँकेमध्ये भरणा करण्यात आली.</v>
+        <v>दिनांक 02.12.2025 रोजी रविवार असल्याने जमा झालेली रक्कम ही सोमवार दिनांक 03.12.2025 रोजी बँकेमध्ये भरणा करण्यात आली.</v>
       </c>
       <c r="G8" t="str">
         <v>2025-12-23</v>
@@ -594,7 +594,7 @@
         <v>010965012-Medha Sub Division Office Coll.</v>
       </c>
       <c r="C9" t="str">
-        <v>NEFT</v>
+        <v>Cheque</v>
       </c>
       <c r="D9" t="str">
         <v/>
@@ -603,7 +603,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="str">
-        <v>दिनांक __ रोजी रविवार असल्याने जमा झालेली रक्कम ही सोमवार दिनांक 03.12.2025 रोजी बँकेमध्ये भरणा करण्यात आली.</v>
+        <v>दिनांक 02.12.2025 रोजी रविवार असल्याने जमा झालेली रक्कम ही सोमवार दिनांक 03.12.2025 रोजी बँकेमध्ये भरणा करण्यात आली.</v>
       </c>
       <c r="G9" t="str">
         <v>2025-12-23</v>
@@ -617,7 +617,7 @@
         <v>010965012-Medha Sub Division Office Coll.</v>
       </c>
       <c r="C10" t="str">
-        <v>Total</v>
+        <v>NEFT</v>
       </c>
       <c r="D10" t="str">
         <v/>
@@ -626,7 +626,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="str">
-        <v>दिनांक __ रोजी रविवार असल्याने जमा झालेली रक्कम ही सोमवार दिनांक 03.12.2025 रोजी बँकेमध्ये भरणा करण्यात आली.</v>
+        <v>दिनांक 02.12.2025 रोजी रविवार असल्याने जमा झालेली रक्कम ही सोमवार दिनांक 03.12.2025 रोजी बँकेमध्ये भरणा करण्यात आली.</v>
       </c>
       <c r="G10" t="str">
         <v>2025-12-23</v>
@@ -640,7 +640,7 @@
         <v>010965012-Medha Sub Division Office Coll.</v>
       </c>
       <c r="C11" t="str">
-        <v>Cash</v>
+        <v>Total</v>
       </c>
       <c r="D11" t="str">
         <v/>

</xml_diff>

<commit_message>
Update Bank Deposit data - 2025-12-23T09:57:08.642Z
</commit_message>
<xml_diff>
--- a/Bank_Deposit.xlsx
+++ b/Bank_Deposit.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -551,10 +551,10 @@
         <v>Cash</v>
       </c>
       <c r="D7" t="str">
-        <v>2025-12-03</v>
+        <v/>
       </c>
       <c r="E7">
-        <v>8770</v>
+        <v>0</v>
       </c>
       <c r="F7" t="str">
         <v>दिनांक 02.12.2025 रोजी रविवार असल्याने जमा झालेली रक्कम ही सोमवार दिनांक 03.12.2025 रोजी बँकेमध्ये भरणा करण्यात आली.</v>
@@ -655,9 +655,101 @@
         <v>2025-12-23</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>02-12-2025</v>
+      </c>
+      <c r="B12" t="str">
+        <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D12" t="str">
+        <v>2025-12-02</v>
+      </c>
+      <c r="E12">
+        <v>70200</v>
+      </c>
+      <c r="F12" t="str">
+        <v/>
+      </c>
+      <c r="G12" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>02-12-2025</v>
+      </c>
+      <c r="B13" t="str">
+        <v>020965019-SHRI DATTATRAY MAHARAJ KALAMBE SAH. PAT. LTD.DAPAWADI</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D13" t="str">
+        <v>2025-12-02</v>
+      </c>
+      <c r="E13">
+        <v>17700</v>
+      </c>
+      <c r="F13" t="str">
+        <v/>
+      </c>
+      <c r="G13" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>02-12-2025</v>
+      </c>
+      <c r="B14" t="str">
+        <v>020965020-KAI.LALSINGRAO BAPUSO SHINDE SAH.PAT.LTD.,KUDAL BR.SAYGAON</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D14" t="str">
+        <v>2025-12-02</v>
+      </c>
+      <c r="E14">
+        <v>13010</v>
+      </c>
+      <c r="F14" t="str">
+        <v/>
+      </c>
+      <c r="G14" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>02-12-2025</v>
+      </c>
+      <c r="B15" t="str">
+        <v>010965012-Medha Sub Division Office Coll.</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D15" t="str">
+        <v/>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="str">
+        <v>दिनांक 02.12.2025 रोजी रविवार असल्याने जमा झालेली रक्कम ही सोमवार दिनांक 03.12.2025 रोजी बँकेमध्ये भरणा करण्यात आली.</v>
+      </c>
+      <c r="G15" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G15"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Bank Deposit data - 2025-12-23T10:14:24.863Z
</commit_message>
<xml_diff>
--- a/Bank_Deposit.xlsx
+++ b/Bank_Deposit.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -689,10 +689,10 @@
         <v>Cash</v>
       </c>
       <c r="D13" t="str">
-        <v/>
+        <v>2025-12-03</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>8770</v>
       </c>
       <c r="F13" t="str">
         <v>दिनांक 02.12.2025 रोजी मेढा नगरपंचायत मतदान निमित्त स्थानिक बँकेला सुट्टी असल्याने हे कलेक्शन दिनांक 03.12.2025 रोजी बँकेमध्ये जमा करण्यात आले.</v>
@@ -724,9 +724,124 @@
         <v>2025-12-23</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>03-12-2025</v>
+      </c>
+      <c r="B15" t="str">
+        <v>010965012-Medha Sub Division Office Coll.</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D15" t="str">
+        <v>2025-12-03</v>
+      </c>
+      <c r="E15">
+        <v>23120</v>
+      </c>
+      <c r="F15" t="str">
+        <v/>
+      </c>
+      <c r="G15" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>03-12-2025</v>
+      </c>
+      <c r="B16" t="str">
+        <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D16" t="str">
+        <v>2025-12-03</v>
+      </c>
+      <c r="E16">
+        <v>78770</v>
+      </c>
+      <c r="F16" t="str">
+        <v/>
+      </c>
+      <c r="G16" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>03-12-2025</v>
+      </c>
+      <c r="B17" t="str">
+        <v>020965018-Kai Lalsingrao Shinde Gr.Big.Sheti Sah.Pat.Ltd. Br. Medha</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D17" t="str">
+        <v>2025-12-03</v>
+      </c>
+      <c r="E17">
+        <v>64270</v>
+      </c>
+      <c r="F17" t="str">
+        <v/>
+      </c>
+      <c r="G17" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>03-12-2025</v>
+      </c>
+      <c r="B18" t="str">
+        <v>020965019-SHRI DATTATRAY MAHARAJ KALAMBE SAH. PAT. LTD.DAPAWADI</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D18" t="str">
+        <v>2025-12-03</v>
+      </c>
+      <c r="E18">
+        <v>16600</v>
+      </c>
+      <c r="F18" t="str">
+        <v/>
+      </c>
+      <c r="G18" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>03-12-2025</v>
+      </c>
+      <c r="B19" t="str">
+        <v>020965020-KAI.LALSINGRAO BAPUSO SHINDE SAH.PAT.LTD.,KUDAL BR.SAYGAON</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D19" t="str">
+        <v>2025-12-03</v>
+      </c>
+      <c r="E19">
+        <v>11350</v>
+      </c>
+      <c r="F19" t="str">
+        <v/>
+      </c>
+      <c r="G19" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G19"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Bank Deposit data - 2025-12-23T11:03:55.260Z
</commit_message>
<xml_diff>
--- a/Bank_Deposit.xlsx
+++ b/Bank_Deposit.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -839,9 +839,101 @@
         <v>2025-12-23</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>04-12-2025</v>
+      </c>
+      <c r="B20" t="str">
+        <v>010965012-Medha Sub Division Office Coll.</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D20" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="E20">
+        <v>16550</v>
+      </c>
+      <c r="F20" t="str">
+        <v/>
+      </c>
+      <c r="G20" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>04-12-2025</v>
+      </c>
+      <c r="B21" t="str">
+        <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D21" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="E21">
+        <v>71040</v>
+      </c>
+      <c r="F21" t="str">
+        <v/>
+      </c>
+      <c r="G21" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>04-12-2025</v>
+      </c>
+      <c r="B22" t="str">
+        <v>020965018-Kai Lalsingrao Shinde Gr.Big.Sheti Sah.Pat.Ltd. Br. Medha</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D22" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="E22">
+        <v>31720</v>
+      </c>
+      <c r="F22" t="str">
+        <v/>
+      </c>
+      <c r="G22" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>04-12-2025</v>
+      </c>
+      <c r="B23" t="str">
+        <v>020965019-SHRI DATTATRAY MAHARAJ KALAMBE SAH. PAT. LTD.DAPAWADI</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D23" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="E23">
+        <v>25700</v>
+      </c>
+      <c r="F23" t="str">
+        <v/>
+      </c>
+      <c r="G23" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G19"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G23"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Bank Deposit data - 2025-12-23T11:06:35.081Z
</commit_message>
<xml_diff>
--- a/Bank_Deposit.xlsx
+++ b/Bank_Deposit.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -931,9 +931,101 @@
         <v>2025-12-23</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>05-12-2025</v>
+      </c>
+      <c r="B24" t="str">
+        <v>010965012-Medha Sub Division Office Coll.</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D24" t="str">
+        <v>2025-12-05</v>
+      </c>
+      <c r="E24">
+        <v>28180</v>
+      </c>
+      <c r="F24" t="str">
+        <v/>
+      </c>
+      <c r="G24" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>05-12-2025</v>
+      </c>
+      <c r="B25" t="str">
+        <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D25" t="str">
+        <v>2025-12-05</v>
+      </c>
+      <c r="E25">
+        <v>59730</v>
+      </c>
+      <c r="F25" t="str">
+        <v/>
+      </c>
+      <c r="G25" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>05-12-2025</v>
+      </c>
+      <c r="B26" t="str">
+        <v>020965018-Kai Lalsingrao Shinde Gr.Big.Sheti Sah.Pat.Ltd. Br. Medha</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D26" t="str">
+        <v>2025-12-05</v>
+      </c>
+      <c r="E26">
+        <v>32740</v>
+      </c>
+      <c r="F26" t="str">
+        <v/>
+      </c>
+      <c r="G26" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>05-12-2025</v>
+      </c>
+      <c r="B27" t="str">
+        <v>020965021-KAI.LALSINGRAO BAPUSO SHINDE SAH.PAT.LTD.,KUDAL, BR.KARAHAR</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D27" t="str">
+        <v>2025-12-05</v>
+      </c>
+      <c r="E27">
+        <v>4020</v>
+      </c>
+      <c r="F27" t="str">
+        <v/>
+      </c>
+      <c r="G27" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G23"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G27"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Bank Deposit data - 2025-12-23T11:15:35.947Z
</commit_message>
<xml_diff>
--- a/Bank_Deposit.xlsx
+++ b/Bank_Deposit.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -933,19 +933,19 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>05-12-2025</v>
+        <v>06-12-2025</v>
       </c>
       <c r="B24" t="str">
-        <v>010965012-Medha Sub Division Office Coll.</v>
+        <v>020965018-Kai Lalsingrao Shinde Gr.Big.Sheti Sah.Pat.Ltd. Br. Medha</v>
       </c>
       <c r="C24" t="str">
         <v>Cash</v>
       </c>
       <c r="D24" t="str">
-        <v>2025-12-05</v>
+        <v>2025-12-06</v>
       </c>
       <c r="E24">
-        <v>28180</v>
+        <v>23170</v>
       </c>
       <c r="F24" t="str">
         <v/>
@@ -956,7 +956,7 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>05-12-2025</v>
+        <v>06-12-2025</v>
       </c>
       <c r="B25" t="str">
         <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
@@ -965,67 +965,21 @@
         <v>Cash</v>
       </c>
       <c r="D25" t="str">
-        <v>2025-12-05</v>
+        <v>2025-12-06</v>
       </c>
       <c r="E25">
-        <v>59730</v>
+        <v>47860</v>
       </c>
       <c r="F25" t="str">
         <v/>
       </c>
       <c r="G25" t="str">
-        <v>2025-12-23</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="str">
-        <v>05-12-2025</v>
-      </c>
-      <c r="B26" t="str">
-        <v>020965018-Kai Lalsingrao Shinde Gr.Big.Sheti Sah.Pat.Ltd. Br. Medha</v>
-      </c>
-      <c r="C26" t="str">
-        <v>Cash</v>
-      </c>
-      <c r="D26" t="str">
-        <v>2025-12-05</v>
-      </c>
-      <c r="E26">
-        <v>32740</v>
-      </c>
-      <c r="F26" t="str">
-        <v/>
-      </c>
-      <c r="G26" t="str">
-        <v>2025-12-23</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="str">
-        <v>05-12-2025</v>
-      </c>
-      <c r="B27" t="str">
-        <v>020965021-KAI.LALSINGRAO BAPUSO SHINDE SAH.PAT.LTD.,KUDAL, BR.KARAHAR</v>
-      </c>
-      <c r="C27" t="str">
-        <v>Cash</v>
-      </c>
-      <c r="D27" t="str">
-        <v>2025-12-05</v>
-      </c>
-      <c r="E27">
-        <v>4020</v>
-      </c>
-      <c r="F27" t="str">
-        <v/>
-      </c>
-      <c r="G27" t="str">
         <v>2025-12-23</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G27"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G25"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Bank Deposit data - 2025-12-23T11:23:46.568Z
</commit_message>
<xml_diff>
--- a/Bank_Deposit.xlsx
+++ b/Bank_Deposit.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -977,9 +977,193 @@
         <v>2025-12-23</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>05-12-2025</v>
+      </c>
+      <c r="B26" t="str">
+        <v>010965012-Medha Sub Division Office Coll.</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D26" t="str">
+        <v>2025-12-05</v>
+      </c>
+      <c r="E26">
+        <v>28180</v>
+      </c>
+      <c r="F26" t="str">
+        <v/>
+      </c>
+      <c r="G26" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>05-12-2025</v>
+      </c>
+      <c r="B27" t="str">
+        <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D27" t="str">
+        <v>2025-12-05</v>
+      </c>
+      <c r="E27">
+        <v>59730</v>
+      </c>
+      <c r="F27" t="str">
+        <v>रद्द झालेल्या दोन रिसिटची रक्कम रु 2020.00 एवढी बँकेमार्फत नजरचुकीने भरली गेल्याने, रु 2020.00  एवढी रक्कम दिनांक 06.12.2025 च्या एकूण कलेक्शन मधून कमी भरणार असल्याचे सांगण्यात आले. ( आज रोजीचे एकूण कलेक्शन 57110.00 असे आहे )</v>
+      </c>
+      <c r="G27" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>05-12-2025</v>
+      </c>
+      <c r="B28" t="str">
+        <v>020965018-Kai Lalsingrao Shinde Gr.Big.Sheti Sah.Pat.Ltd. Br. Medha</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D28" t="str">
+        <v>2025-12-05</v>
+      </c>
+      <c r="E28">
+        <v>32740</v>
+      </c>
+      <c r="F28" t="str">
+        <v/>
+      </c>
+      <c r="G28" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>05-12-2025</v>
+      </c>
+      <c r="B29" t="str">
+        <v>020965021-KAI.LALSINGRAO BAPUSO SHINDE SAH.PAT.LTD.,KUDAL, BR.KARAHAR</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D29" t="str">
+        <v>2025-12-05</v>
+      </c>
+      <c r="E29">
+        <v>4020</v>
+      </c>
+      <c r="F29" t="str">
+        <v/>
+      </c>
+      <c r="G29" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>05-12-2025</v>
+      </c>
+      <c r="B30" t="str">
+        <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
+      </c>
+      <c r="C30" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D30" t="str">
+        <v/>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="str">
+        <v>रद्द झालेल्या दोन रिसिटची रक्कम रु 2020.00 एवढी बँकेमार्फत नजरचुकीने भरली गेल्याने, रु 2020.00  एवढी रक्कम दिनांक 06.12.2025 च्या एकूण कलेक्शन मधून कमी भरणार असल्याचे सांगण्यात आले. ( आज रोजीचे एकूण कलेक्शन 57110.00 असे आहे )</v>
+      </c>
+      <c r="G30" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>05-12-2025</v>
+      </c>
+      <c r="B31" t="str">
+        <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="D31" t="str">
+        <v/>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" t="str">
+        <v>रद्द झालेल्या दोन रिसिटची रक्कम रु 2020.00 एवढी बँकेमार्फत नजरचुकीने भरली गेल्याने, रु 2020.00  एवढी रक्कम दिनांक 06.12.2025 च्या एकूण कलेक्शन मधून कमी भरणार असल्याचे सांगण्यात आले. ( आज रोजीचे एकूण कलेक्शन 57110.00 असे आहे )</v>
+      </c>
+      <c r="G31" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>05-12-2025</v>
+      </c>
+      <c r="B32" t="str">
+        <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
+      </c>
+      <c r="C32" t="str">
+        <v>NEFT</v>
+      </c>
+      <c r="D32" t="str">
+        <v/>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" t="str">
+        <v>रद्द झालेल्या दोन रिसिटची रक्कम रु 2020.00 एवढी बँकेमार्फत नजरचुकीने भरली गेल्याने, रु 2020.00  एवढी रक्कम दिनांक 06.12.2025 च्या एकूण कलेक्शन मधून कमी भरणार असल्याचे सांगण्यात आले. ( आज रोजीचे एकूण कलेक्शन 57110.00 असे आहे )</v>
+      </c>
+      <c r="G32" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>05-12-2025</v>
+      </c>
+      <c r="B33" t="str">
+        <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
+      </c>
+      <c r="C33" t="str">
+        <v>Total</v>
+      </c>
+      <c r="D33" t="str">
+        <v/>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" t="str">
+        <v>रद्द झालेल्या दोन रिसिटची रक्कम रु 2020.00 एवढी बँकेमार्फत नजरचुकीने भरली गेल्याने, रु 2020.00  एवढी रक्कम दिनांक 06.12.2025 च्या एकूण कलेक्शन मधून कमी भरणार असल्याचे सांगण्यात आले. ( आज रोजीचे एकूण कलेक्शन 57110.00 असे आहे )</v>
+      </c>
+      <c r="G33" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G25"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G33"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Bank Deposit data - 2025-12-23T11:26:27.967Z
</commit_message>
<xml_diff>
--- a/Bank_Deposit.xlsx
+++ b/Bank_Deposit.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1005,7 +1005,7 @@
         <v>05-12-2025</v>
       </c>
       <c r="B27" t="str">
-        <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
+        <v>020965018-Kai Lalsingrao Shinde Gr.Big.Sheti Sah.Pat.Ltd. Br. Medha</v>
       </c>
       <c r="C27" t="str">
         <v>Cash</v>
@@ -1014,10 +1014,10 @@
         <v>2025-12-05</v>
       </c>
       <c r="E27">
-        <v>59730</v>
+        <v>32740</v>
       </c>
       <c r="F27" t="str">
-        <v>रद्द झालेल्या दोन रिसिटची रक्कम रु 2020.00 एवढी बँकेमार्फत नजरचुकीने भरली गेल्याने, रु 2020.00  एवढी रक्कम दिनांक 06.12.2025 च्या एकूण कलेक्शन मधून कमी भरणार असल्याचे सांगण्यात आले. ( आज रोजीचे एकूण कलेक्शन 57110.00 असे आहे )</v>
+        <v/>
       </c>
       <c r="G27" t="str">
         <v>2025-12-23</v>
@@ -1028,7 +1028,7 @@
         <v>05-12-2025</v>
       </c>
       <c r="B28" t="str">
-        <v>020965018-Kai Lalsingrao Shinde Gr.Big.Sheti Sah.Pat.Ltd. Br. Medha</v>
+        <v>020965021-KAI.LALSINGRAO BAPUSO SHINDE SAH.PAT.LTD.,KUDAL, BR.KARAHAR</v>
       </c>
       <c r="C28" t="str">
         <v>Cash</v>
@@ -1037,7 +1037,7 @@
         <v>2025-12-05</v>
       </c>
       <c r="E28">
-        <v>32740</v>
+        <v>4020</v>
       </c>
       <c r="F28" t="str">
         <v/>
@@ -1051,19 +1051,19 @@
         <v>05-12-2025</v>
       </c>
       <c r="B29" t="str">
-        <v>020965021-KAI.LALSINGRAO BAPUSO SHINDE SAH.PAT.LTD.,KUDAL, BR.KARAHAR</v>
+        <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
       </c>
       <c r="C29" t="str">
-        <v>Cash</v>
+        <v>Cheque</v>
       </c>
       <c r="D29" t="str">
-        <v>2025-12-05</v>
+        <v/>
       </c>
       <c r="E29">
-        <v>4020</v>
+        <v>0</v>
       </c>
       <c r="F29" t="str">
-        <v/>
+        <v>रद्द झालेल्या दोन रिसिटची रक्कम रु 2020.00 एवढी बँकेमार्फत नजरचुकीने भरली गेल्याने, रु 2020.00  एवढी रक्कम दिनांक 06.12.2025 च्या एकूण कलेक्शन मधून कमी भरणार असल्याचे सांगण्यात आले. ( आज रोजीचे एकूण कलेक्शन 57110.00 असे आहे )</v>
       </c>
       <c r="G29" t="str">
         <v>2025-12-23</v>
@@ -1077,7 +1077,7 @@
         <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
       </c>
       <c r="C30" t="str">
-        <v>Cash</v>
+        <v>NEFT</v>
       </c>
       <c r="D30" t="str">
         <v/>
@@ -1100,7 +1100,7 @@
         <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
       </c>
       <c r="C31" t="str">
-        <v>Cheque</v>
+        <v>Total</v>
       </c>
       <c r="D31" t="str">
         <v/>
@@ -1123,13 +1123,13 @@
         <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
       </c>
       <c r="C32" t="str">
-        <v>NEFT</v>
+        <v>Cash</v>
       </c>
       <c r="D32" t="str">
-        <v/>
+        <v>2025-12-05</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>59730</v>
       </c>
       <c r="F32" t="str">
         <v>रद्द झालेल्या दोन रिसिटची रक्कम रु 2020.00 एवढी बँकेमार्फत नजरचुकीने भरली गेल्याने, रु 2020.00  एवढी रक्कम दिनांक 06.12.2025 च्या एकूण कलेक्शन मधून कमी भरणार असल्याचे सांगण्यात आले. ( आज रोजीचे एकूण कलेक्शन 57110.00 असे आहे )</v>
@@ -1138,32 +1138,9 @@
         <v>2025-12-23</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="str">
-        <v>05-12-2025</v>
-      </c>
-      <c r="B33" t="str">
-        <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
-      </c>
-      <c r="C33" t="str">
-        <v>Total</v>
-      </c>
-      <c r="D33" t="str">
-        <v/>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33" t="str">
-        <v>रद्द झालेल्या दोन रिसिटची रक्कम रु 2020.00 एवढी बँकेमार्फत नजरचुकीने भरली गेल्याने, रु 2020.00  एवढी रक्कम दिनांक 06.12.2025 च्या एकूण कलेक्शन मधून कमी भरणार असल्याचे सांगण्यात आले. ( आज रोजीचे एकूण कलेक्शन 57110.00 असे आहे )</v>
-      </c>
-      <c r="G33" t="str">
-        <v>2025-12-23</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G33"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G32"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Bank Deposit data - 2025-12-23T11:31:36.662Z
</commit_message>
<xml_diff>
--- a/Bank_Deposit.xlsx
+++ b/Bank_Deposit.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1126,10 +1126,10 @@
         <v>Cash</v>
       </c>
       <c r="D32" t="str">
-        <v>2025-12-05</v>
+        <v/>
       </c>
       <c r="E32">
-        <v>59730</v>
+        <v>0</v>
       </c>
       <c r="F32" t="str">
         <v>रद्द झालेल्या दोन रिसिटची रक्कम रु 2020.00 एवढी बँकेमार्फत नजरचुकीने भरली गेल्याने, रु 2020.00  एवढी रक्कम दिनांक 06.12.2025 च्या एकूण कलेक्शन मधून कमी भरणार असल्याचे सांगण्यात आले. ( आज रोजीचे एकूण कलेक्शन 57110.00 असे आहे )</v>
@@ -1138,9 +1138,101 @@
         <v>2025-12-23</v>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>08-12-2025</v>
+      </c>
+      <c r="B33" t="str">
+        <v>010965012-Medha Sub Division Office Coll.</v>
+      </c>
+      <c r="C33" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D33" t="str">
+        <v>2025-12-08</v>
+      </c>
+      <c r="E33">
+        <v>44300</v>
+      </c>
+      <c r="F33" t="str">
+        <v/>
+      </c>
+      <c r="G33" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>08-12-2025</v>
+      </c>
+      <c r="B34" t="str">
+        <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D34" t="str">
+        <v>2025-12-08</v>
+      </c>
+      <c r="E34">
+        <v>64020</v>
+      </c>
+      <c r="F34" t="str">
+        <v/>
+      </c>
+      <c r="G34" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>08-12-2025</v>
+      </c>
+      <c r="B35" t="str">
+        <v>020965018-Kai Lalsingrao Shinde Gr.Big.Sheti Sah.Pat.Ltd. Br. Medha</v>
+      </c>
+      <c r="C35" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D35" t="str">
+        <v>2025-12-08</v>
+      </c>
+      <c r="E35">
+        <v>54910</v>
+      </c>
+      <c r="F35" t="str">
+        <v/>
+      </c>
+      <c r="G35" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>08-12-2025</v>
+      </c>
+      <c r="B36" t="str">
+        <v>020965019-SHRI DATTATRAY MAHARAJ KALAMBE SAH. PAT. LTD.DAPAWADI</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Cash</v>
+      </c>
+      <c r="D36" t="str">
+        <v>2025-12-08</v>
+      </c>
+      <c r="E36">
+        <v>16290</v>
+      </c>
+      <c r="F36" t="str">
+        <v/>
+      </c>
+      <c r="G36" t="str">
+        <v>2025-12-23</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G32"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G36"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Bank Deposit data - 2025-12-23T11:31:48.817Z
</commit_message>
<xml_diff>
--- a/Bank_Deposit.xlsx
+++ b/Bank_Deposit.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1126,10 +1126,10 @@
         <v>Cash</v>
       </c>
       <c r="D32" t="str">
-        <v/>
+        <v>2025-12-05</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>59730</v>
       </c>
       <c r="F32" t="str">
         <v>रद्द झालेल्या दोन रिसिटची रक्कम रु 2020.00 एवढी बँकेमार्फत नजरचुकीने भरली गेल्याने, रु 2020.00  एवढी रक्कम दिनांक 06.12.2025 च्या एकूण कलेक्शन मधून कमी भरणार असल्याचे सांगण्यात आले. ( आज रोजीचे एकूण कलेक्शन 57110.00 असे आहे )</v>
@@ -1138,101 +1138,9 @@
         <v>2025-12-23</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="str">
-        <v>08-12-2025</v>
-      </c>
-      <c r="B33" t="str">
-        <v>010965012-Medha Sub Division Office Coll.</v>
-      </c>
-      <c r="C33" t="str">
-        <v>Cash</v>
-      </c>
-      <c r="D33" t="str">
-        <v>2025-12-08</v>
-      </c>
-      <c r="E33">
-        <v>44300</v>
-      </c>
-      <c r="F33" t="str">
-        <v/>
-      </c>
-      <c r="G33" t="str">
-        <v>2025-12-23</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="str">
-        <v>08-12-2025</v>
-      </c>
-      <c r="B34" t="str">
-        <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
-      </c>
-      <c r="C34" t="str">
-        <v>Cash</v>
-      </c>
-      <c r="D34" t="str">
-        <v>2025-12-08</v>
-      </c>
-      <c r="E34">
-        <v>64020</v>
-      </c>
-      <c r="F34" t="str">
-        <v/>
-      </c>
-      <c r="G34" t="str">
-        <v>2025-12-23</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="str">
-        <v>08-12-2025</v>
-      </c>
-      <c r="B35" t="str">
-        <v>020965018-Kai Lalsingrao Shinde Gr.Big.Sheti Sah.Pat.Ltd. Br. Medha</v>
-      </c>
-      <c r="C35" t="str">
-        <v>Cash</v>
-      </c>
-      <c r="D35" t="str">
-        <v>2025-12-08</v>
-      </c>
-      <c r="E35">
-        <v>54910</v>
-      </c>
-      <c r="F35" t="str">
-        <v/>
-      </c>
-      <c r="G35" t="str">
-        <v>2025-12-23</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="str">
-        <v>08-12-2025</v>
-      </c>
-      <c r="B36" t="str">
-        <v>020965019-SHRI DATTATRAY MAHARAJ KALAMBE SAH. PAT. LTD.DAPAWADI</v>
-      </c>
-      <c r="C36" t="str">
-        <v>Cash</v>
-      </c>
-      <c r="D36" t="str">
-        <v>2025-12-08</v>
-      </c>
-      <c r="E36">
-        <v>16290</v>
-      </c>
-      <c r="F36" t="str">
-        <v/>
-      </c>
-      <c r="G36" t="str">
-        <v>2025-12-23</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G36"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G32"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Bank Deposit data - 2025-12-24T09:56:21.017Z
</commit_message>
<xml_diff>
--- a/Bank_Deposit.xlsx
+++ b/Bank_Deposit.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -956,22 +956,22 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>06-12-2025</v>
+        <v>05-12-2025</v>
       </c>
       <c r="B25" t="str">
-        <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
+        <v>010965012-Medha Sub Division Office Coll.</v>
       </c>
       <c r="C25" t="str">
         <v>Cash</v>
       </c>
       <c r="D25" t="str">
-        <v>2025-12-06</v>
+        <v>2025-12-05</v>
       </c>
       <c r="E25">
-        <v>47860</v>
+        <v>28180</v>
       </c>
       <c r="F25" t="str">
-        <v>दिनांक 05.12.2025 रोजी रद्द झालेल्या दोन रिसिटची रक्कम रु 2020.00 एवढी बँकेमार्फत नजरचुकीने भरली गेल्याने, रु 2020.00 एवढी रक्कम दिनांक 06.12.2025 च्या एकूण कलेक्शन मधून कमी भरलेली आहे.</v>
+        <v/>
       </c>
       <c r="G25" t="str">
         <v>2025-12-23</v>
@@ -982,7 +982,7 @@
         <v>05-12-2025</v>
       </c>
       <c r="B26" t="str">
-        <v>010965012-Medha Sub Division Office Coll.</v>
+        <v>020965018-Kai Lalsingrao Shinde Gr.Big.Sheti Sah.Pat.Ltd. Br. Medha</v>
       </c>
       <c r="C26" t="str">
         <v>Cash</v>
@@ -991,7 +991,7 @@
         <v>2025-12-05</v>
       </c>
       <c r="E26">
-        <v>28180</v>
+        <v>32740</v>
       </c>
       <c r="F26" t="str">
         <v/>
@@ -1005,7 +1005,7 @@
         <v>05-12-2025</v>
       </c>
       <c r="B27" t="str">
-        <v>020965018-Kai Lalsingrao Shinde Gr.Big.Sheti Sah.Pat.Ltd. Br. Medha</v>
+        <v>020965021-KAI.LALSINGRAO BAPUSO SHINDE SAH.PAT.LTD.,KUDAL, BR.KARAHAR</v>
       </c>
       <c r="C27" t="str">
         <v>Cash</v>
@@ -1014,7 +1014,7 @@
         <v>2025-12-05</v>
       </c>
       <c r="E27">
-        <v>32740</v>
+        <v>4020</v>
       </c>
       <c r="F27" t="str">
         <v/>
@@ -1028,19 +1028,19 @@
         <v>05-12-2025</v>
       </c>
       <c r="B28" t="str">
-        <v>020965021-KAI.LALSINGRAO BAPUSO SHINDE SAH.PAT.LTD.,KUDAL, BR.KARAHAR</v>
+        <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
       </c>
       <c r="C28" t="str">
-        <v>Cash</v>
+        <v>Cheque</v>
       </c>
       <c r="D28" t="str">
-        <v>2025-12-05</v>
+        <v/>
       </c>
       <c r="E28">
-        <v>4020</v>
+        <v>0</v>
       </c>
       <c r="F28" t="str">
-        <v/>
+        <v>रद्द झालेल्या दोन रिसिटची रक्कम रु 2020.00 एवढी बँकेमार्फत नजरचुकीने भरली गेल्याने, रु 2020.00  एवढी रक्कम दिनांक 06.12.2025 च्या एकूण कलेक्शन मधून कमी भरणार असल्याचे सांगण्यात आले. ( आज रोजीचे एकूण कलेक्शन 57110.00 असे आहे )</v>
       </c>
       <c r="G28" t="str">
         <v>2025-12-23</v>
@@ -1054,7 +1054,7 @@
         <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
       </c>
       <c r="C29" t="str">
-        <v>Cheque</v>
+        <v>NEFT</v>
       </c>
       <c r="D29" t="str">
         <v/>
@@ -1077,7 +1077,7 @@
         <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
       </c>
       <c r="C30" t="str">
-        <v>NEFT</v>
+        <v>Total</v>
       </c>
       <c r="D30" t="str">
         <v/>
@@ -1100,13 +1100,13 @@
         <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
       </c>
       <c r="C31" t="str">
-        <v>Total</v>
+        <v>Cash</v>
       </c>
       <c r="D31" t="str">
-        <v/>
+        <v>2025-12-05</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>59730</v>
       </c>
       <c r="F31" t="str">
         <v>रद्द झालेल्या दोन रिसिटची रक्कम रु 2020.00 एवढी बँकेमार्फत नजरचुकीने भरली गेल्याने, रु 2020.00  एवढी रक्कम दिनांक 06.12.2025 च्या एकूण कलेक्शन मधून कमी भरणार असल्याचे सांगण्यात आले. ( आज रोजीचे एकूण कलेक्शन 57110.00 असे आहे )</v>
@@ -1140,22 +1140,22 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>05-12-2025</v>
+        <v>06-12-2025</v>
       </c>
       <c r="B33" t="str">
         <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
       </c>
       <c r="C33" t="str">
-        <v>Cash</v>
+        <v>Cheque</v>
       </c>
       <c r="D33" t="str">
-        <v>2025-12-05</v>
+        <v/>
       </c>
       <c r="E33">
-        <v>59730</v>
+        <v>0</v>
       </c>
       <c r="F33" t="str">
-        <v>रद्द झालेल्या दोन रिसिटची रक्कम रु 2020.00 एवढी बँकेमार्फत नजरचुकीने भरली गेल्याने, रु 2020.00  एवढी रक्कम दिनांक 06.12.2025 च्या एकूण कलेक्शन मधून कमी भरणार असल्याचे सांगण्यात आले. ( आज रोजीचे एकूण कलेक्शन 57110.00 असे आहे )</v>
+        <v>दिनांक 05.12.2025 रोजी रद्द झालेल्या दोन रिसिटची रक्कम रु 2020.00 एवढी बँकेमार्फत नजरचुकीने भरली गेल्याने, रु 2020.00 एवढी रक्कम दिनांक 06.12.2025 च्या एकूण कलेक्शन मधून कमी भरलेली आहे.</v>
       </c>
       <c r="G33" t="str">
         <v>2025-12-23</v>
@@ -1169,7 +1169,7 @@
         <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
       </c>
       <c r="C34" t="str">
-        <v>Cash</v>
+        <v>NEFT</v>
       </c>
       <c r="D34" t="str">
         <v/>
@@ -1192,7 +1192,7 @@
         <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
       </c>
       <c r="C35" t="str">
-        <v>Cheque</v>
+        <v>Total</v>
       </c>
       <c r="D35" t="str">
         <v/>
@@ -1215,47 +1215,24 @@
         <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
       </c>
       <c r="C36" t="str">
-        <v>NEFT</v>
+        <v>Cash</v>
       </c>
       <c r="D36" t="str">
-        <v/>
+        <v>2025-12-06</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>47860</v>
       </c>
       <c r="F36" t="str">
         <v>दिनांक 05.12.2025 रोजी रद्द झालेल्या दोन रिसिटची रक्कम रु 2020.00 एवढी बँकेमार्फत नजरचुकीने भरली गेल्याने, रु 2020.00 एवढी रक्कम दिनांक 06.12.2025 च्या एकूण कलेक्शन मधून कमी भरलेली आहे.</v>
       </c>
       <c r="G36" t="str">
-        <v>2025-12-23</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="str">
-        <v>06-12-2025</v>
-      </c>
-      <c r="B37" t="str">
-        <v>020965017-Kai Lalsingrao Shinde Gr.Bid.S.S.Pat.Ltd Kudal Br. Kudal</v>
-      </c>
-      <c r="C37" t="str">
-        <v>Total</v>
-      </c>
-      <c r="D37" t="str">
-        <v/>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37" t="str">
-        <v>दिनांक 05.12.2025 रोजी रद्द झालेल्या दोन रिसिटची रक्कम रु 2020.00 एवढी बँकेमार्फत नजरचुकीने भरली गेल्याने, रु 2020.00 एवढी रक्कम दिनांक 06.12.2025 च्या एकूण कलेक्शन मधून कमी भरलेली आहे.</v>
-      </c>
-      <c r="G37" t="str">
-        <v>2025-12-23</v>
+        <v>2025-12-24</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G37"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G36"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>